<commit_message>
added party_normalized column for few parties
</commit_message>
<xml_diff>
--- a/clean_rs_parties/rs_clean_blanks.xlsx
+++ b/clean_rs_parties/rs_clean_blanks.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salonibhogale/Documents/GitHub/Rajya-Sabha/clean_rs_parties/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9037AF84-E3A5-474C-9326-8FF377ADF630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="600" windowWidth="20535" windowHeight="9420"/>
+    <workbookView xWindow="5000" yWindow="2060" windowWidth="20540" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rs_clean_blanks" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="233">
   <si>
     <t>no</t>
   </si>
@@ -680,13 +686,49 @@
   </si>
   <si>
     <t>Nagaland People's Council</t>
+  </si>
+  <si>
+    <t>Praja Socialist Party</t>
+  </si>
+  <si>
+    <t>Commmunist Party of India</t>
+  </si>
+  <si>
+    <t>Ganatantra Parishad</t>
+  </si>
+  <si>
+    <t>Peasants and Workers Party</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Shiromani Akali Dal</t>
+  </si>
+  <si>
+    <t>Socialist Party</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Republican Party of India</t>
+  </si>
+  <si>
+    <t>Kisan Mazdoor Praja Party</t>
+  </si>
+  <si>
+    <t>Progressive Independent Party</t>
+  </si>
+  <si>
+    <t>Jan Sangh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -822,8 +864,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1003,6 +1051,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1164,10 +1218,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="14" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1215,6 +1271,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1261,7 +1325,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1293,9 +1357,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1327,6 +1409,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1502,14 +1602,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -1571,6 +1669,9 @@
       <c r="I2" t="s">
         <v>13</v>
       </c>
+      <c r="J2" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
@@ -1600,6 +1701,9 @@
       <c r="I3" t="s">
         <v>13</v>
       </c>
+      <c r="J3" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
@@ -1629,6 +1733,9 @@
       <c r="I4" t="s">
         <v>13</v>
       </c>
+      <c r="J4" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
@@ -1658,6 +1765,9 @@
       <c r="I5" t="s">
         <v>13</v>
       </c>
+      <c r="J5" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
@@ -1687,6 +1797,9 @@
       <c r="I6" t="s">
         <v>22</v>
       </c>
+      <c r="J6" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
@@ -1716,6 +1829,9 @@
       <c r="I7" t="s">
         <v>22</v>
       </c>
+      <c r="J7" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
@@ -1745,6 +1861,9 @@
       <c r="I8" t="s">
         <v>13</v>
       </c>
+      <c r="J8" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
@@ -1774,6 +1893,9 @@
       <c r="I9" t="s">
         <v>13</v>
       </c>
+      <c r="J9" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
@@ -1803,6 +1925,9 @@
       <c r="I10" t="s">
         <v>13</v>
       </c>
+      <c r="J10" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
@@ -1832,6 +1957,9 @@
       <c r="I11" t="s">
         <v>13</v>
       </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
@@ -1861,6 +1989,9 @@
       <c r="I12" t="s">
         <v>13</v>
       </c>
+      <c r="J12" s="3" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
@@ -1890,6 +2021,9 @@
       <c r="I13" t="s">
         <v>13</v>
       </c>
+      <c r="J13" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
@@ -1919,6 +2053,9 @@
       <c r="I14" t="s">
         <v>13</v>
       </c>
+      <c r="J14" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
@@ -1948,6 +2085,9 @@
       <c r="I15" t="s">
         <v>41</v>
       </c>
+      <c r="J15" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
@@ -1977,8 +2117,11 @@
       <c r="I16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>55</v>
       </c>
@@ -2006,8 +2149,11 @@
       <c r="I17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>55</v>
       </c>
@@ -2035,8 +2181,11 @@
       <c r="I18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>103</v>
       </c>
@@ -2064,8 +2213,11 @@
       <c r="I19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>99</v>
       </c>
@@ -2093,8 +2245,11 @@
       <c r="I20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>26</v>
       </c>
@@ -2122,8 +2277,11 @@
       <c r="I21" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>26</v>
       </c>
@@ -2151,8 +2309,11 @@
       <c r="I22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>114</v>
       </c>
@@ -2180,8 +2341,11 @@
       <c r="I23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>141</v>
       </c>
@@ -2209,8 +2373,11 @@
       <c r="I24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>156</v>
       </c>
@@ -2238,8 +2405,11 @@
       <c r="I25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>182</v>
       </c>
@@ -2267,8 +2437,11 @@
       <c r="I26" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>198</v>
       </c>
@@ -2296,8 +2469,11 @@
       <c r="I27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>267</v>
       </c>
@@ -2325,8 +2501,11 @@
       <c r="I28" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="16">
       <c r="A29">
         <v>326</v>
       </c>
@@ -2354,8 +2533,11 @@
       <c r="I29" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>32</v>
       </c>
@@ -2383,8 +2565,11 @@
       <c r="I30" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>52</v>
       </c>
@@ -2412,8 +2597,11 @@
       <c r="I31" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>56</v>
       </c>
@@ -2440,6 +2628,9 @@
       </c>
       <c r="I32" t="s">
         <v>13</v>
+      </c>
+      <c r="J32" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2470,6 +2661,9 @@
       <c r="I33" t="s">
         <v>13</v>
       </c>
+      <c r="J33" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34">
@@ -2499,6 +2693,9 @@
       <c r="I34" t="s">
         <v>41</v>
       </c>
+      <c r="J34" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35">
@@ -2528,6 +2725,9 @@
       <c r="I35" t="s">
         <v>13</v>
       </c>
+      <c r="J35" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36">
@@ -2557,6 +2757,9 @@
       <c r="I36" t="s">
         <v>13</v>
       </c>
+      <c r="J36" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37">
@@ -2586,6 +2789,9 @@
       <c r="I37" t="s">
         <v>22</v>
       </c>
+      <c r="J37" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38">
@@ -2615,6 +2821,9 @@
       <c r="I38" t="s">
         <v>13</v>
       </c>
+      <c r="J38" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39">
@@ -2644,6 +2853,9 @@
       <c r="I39" t="s">
         <v>41</v>
       </c>
+      <c r="J39" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40">
@@ -2737,6 +2949,9 @@
       <c r="I42" t="s">
         <v>13</v>
       </c>
+      <c r="J42" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43">
@@ -2766,6 +2981,9 @@
       <c r="I43" t="s">
         <v>13</v>
       </c>
+      <c r="J43" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44">
@@ -2795,6 +3013,9 @@
       <c r="I44" t="s">
         <v>66</v>
       </c>
+      <c r="J44" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45">
@@ -2824,6 +3045,9 @@
       <c r="I45" t="s">
         <v>13</v>
       </c>
+      <c r="J45" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46">
@@ -2853,6 +3077,9 @@
       <c r="I46" t="s">
         <v>13</v>
       </c>
+      <c r="J46" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47">
@@ -2946,6 +3173,9 @@
       <c r="I49" t="s">
         <v>13</v>
       </c>
+      <c r="J49" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50">
@@ -2975,6 +3205,9 @@
       <c r="I50" t="s">
         <v>13</v>
       </c>
+      <c r="J50" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51">
@@ -3004,6 +3237,9 @@
       <c r="I51" t="s">
         <v>13</v>
       </c>
+      <c r="J51" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52">
@@ -3033,6 +3269,9 @@
       <c r="I52" t="s">
         <v>13</v>
       </c>
+      <c r="J52" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53">
@@ -3062,6 +3301,9 @@
       <c r="I53" t="s">
         <v>13</v>
       </c>
+      <c r="J53" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54">
@@ -3155,6 +3397,9 @@
       <c r="I56" t="s">
         <v>13</v>
       </c>
+      <c r="J56" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57">
@@ -3184,6 +3429,9 @@
       <c r="I57" t="s">
         <v>13</v>
       </c>
+      <c r="J57" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58">
@@ -3213,6 +3461,9 @@
       <c r="I58" t="s">
         <v>13</v>
       </c>
+      <c r="J58" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59">
@@ -3242,6 +3493,9 @@
       <c r="I59" t="s">
         <v>13</v>
       </c>
+      <c r="J59" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60">
@@ -3303,6 +3557,9 @@
       <c r="I61" t="s">
         <v>13</v>
       </c>
+      <c r="J61" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62">
@@ -3332,6 +3589,9 @@
       <c r="I62" t="s">
         <v>13</v>
       </c>
+      <c r="J62" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63">
@@ -3361,6 +3621,9 @@
       <c r="I63" t="s">
         <v>13</v>
       </c>
+      <c r="J63" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64">
@@ -3422,6 +3685,9 @@
       <c r="I65" t="s">
         <v>13</v>
       </c>
+      <c r="J65" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66">
@@ -3483,6 +3749,9 @@
       <c r="I67" t="s">
         <v>13</v>
       </c>
+      <c r="J67" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68">
@@ -3512,6 +3781,9 @@
       <c r="I68" t="s">
         <v>22</v>
       </c>
+      <c r="J68" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69">
@@ -3541,6 +3813,9 @@
       <c r="I69" t="s">
         <v>13</v>
       </c>
+      <c r="J69" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70">
@@ -3570,6 +3845,9 @@
       <c r="I70" t="s">
         <v>13</v>
       </c>
+      <c r="J70" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71">
@@ -3599,6 +3877,9 @@
       <c r="I71" t="s">
         <v>13</v>
       </c>
+      <c r="J71" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72">
@@ -3628,6 +3909,9 @@
       <c r="I72" t="s">
         <v>13</v>
       </c>
+      <c r="J72" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73">
@@ -3657,6 +3941,9 @@
       <c r="I73" t="s">
         <v>13</v>
       </c>
+      <c r="J73" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74">
@@ -3686,6 +3973,9 @@
       <c r="I74" t="s">
         <v>13</v>
       </c>
+      <c r="J74" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75">
@@ -3715,6 +4005,9 @@
       <c r="I75" t="s">
         <v>13</v>
       </c>
+      <c r="J75" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76">
@@ -3744,6 +4037,9 @@
       <c r="I76" t="s">
         <v>13</v>
       </c>
+      <c r="J76" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77">
@@ -3773,6 +4069,9 @@
       <c r="I77" t="s">
         <v>13</v>
       </c>
+      <c r="J77" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78">
@@ -3802,6 +4101,9 @@
       <c r="I78" t="s">
         <v>13</v>
       </c>
+      <c r="J78" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79">
@@ -3831,6 +4133,9 @@
       <c r="I79" t="s">
         <v>13</v>
       </c>
+      <c r="J79" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80">
@@ -3860,8 +4165,11 @@
       <c r="I80" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81">
         <v>100</v>
       </c>
@@ -3889,8 +4197,11 @@
       <c r="I81" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82">
         <v>140</v>
       </c>
@@ -3918,8 +4229,11 @@
       <c r="I82" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="J82" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83">
         <v>183</v>
       </c>
@@ -3947,8 +4261,11 @@
       <c r="I83" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="J83" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84">
         <v>104</v>
       </c>
@@ -3976,8 +4293,11 @@
       <c r="I84" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="J84" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85">
         <v>114</v>
       </c>
@@ -4005,8 +4325,11 @@
       <c r="I85" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="J85" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86">
         <v>116</v>
       </c>
@@ -4034,8 +4357,11 @@
       <c r="I86" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J86" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87">
         <v>116</v>
       </c>
@@ -4063,8 +4389,11 @@
       <c r="I87" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="J87" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88">
         <v>119</v>
       </c>
@@ -4092,8 +4421,11 @@
       <c r="I88" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="J88" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89">
         <v>124</v>
       </c>
@@ -4121,8 +4453,11 @@
       <c r="I89" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="J89" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90">
         <v>147</v>
       </c>
@@ -4150,8 +4485,11 @@
       <c r="I90" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="J90" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91">
         <v>153</v>
       </c>
@@ -4179,8 +4517,11 @@
       <c r="I91" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="J91" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92">
         <v>176</v>
       </c>
@@ -4208,8 +4549,11 @@
       <c r="I92" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="J92" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93">
         <v>176</v>
       </c>
@@ -4237,8 +4581,11 @@
       <c r="I93" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="J93" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94">
         <v>227</v>
       </c>
@@ -4266,8 +4613,11 @@
       <c r="I94" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="J94" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95">
         <v>241</v>
       </c>
@@ -4295,8 +4645,11 @@
       <c r="I95" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="J95" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96">
         <v>305</v>
       </c>
@@ -4323,6 +4676,9 @@
       </c>
       <c r="I96" t="s">
         <v>13</v>
+      </c>
+      <c r="J96" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -4353,6 +4709,9 @@
       <c r="I97" t="s">
         <v>66</v>
       </c>
+      <c r="J97" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98">
@@ -4382,6 +4741,9 @@
       <c r="I98" t="s">
         <v>13</v>
       </c>
+      <c r="J98" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99">
@@ -4443,6 +4805,9 @@
       <c r="I100" t="s">
         <v>13</v>
       </c>
+      <c r="J100" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101">
@@ -4472,6 +4837,9 @@
       <c r="I101" t="s">
         <v>13</v>
       </c>
+      <c r="J101" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102">
@@ -4533,6 +4901,9 @@
       <c r="I103" t="s">
         <v>13</v>
       </c>
+      <c r="J103" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104">
@@ -4684,6 +5055,9 @@
       <c r="I108" t="s">
         <v>41</v>
       </c>
+      <c r="J108" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109">
@@ -4713,6 +5087,9 @@
       <c r="I109" t="s">
         <v>66</v>
       </c>
+      <c r="J109" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="110" spans="1:10">
       <c r="A110">
@@ -4806,6 +5183,9 @@
       <c r="I112" t="s">
         <v>22</v>
       </c>
+      <c r="J112" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="113" spans="1:10">
       <c r="A113">
@@ -4957,6 +5337,9 @@
       <c r="I117" t="s">
         <v>13</v>
       </c>
+      <c r="J117" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="118" spans="1:10">
       <c r="A118">
@@ -5165,7 +5548,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J124"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>